<commit_message>
plus mc Praha 5
</commit_message>
<xml_diff>
--- a/materialy/software-mestskych-casti/2016/prehled-software-mc.xlsx
+++ b/materialy/software-mestskych-casti/2016/prehled-software-mc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Přehledová tabulka" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="97">
   <si>
     <t>městská část </t>
   </si>
@@ -142,6 +142,21 @@
   </si>
   <si>
     <t>Praha 6</t>
+  </si>
+  <si>
+    <t>Datacentrum2</t>
+  </si>
+  <si>
+    <t>Materiály RMČ</t>
+  </si>
+  <si>
+    <t>ISMA</t>
+  </si>
+  <si>
+    <t>VERA</t>
+  </si>
+  <si>
+    <t>VISA</t>
   </si>
   <si>
     <t>Praha 7</t>
@@ -546,8 +561,8 @@
   </sheetPr>
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -736,7 +751,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="Q6" s="5"/>
     </row>
@@ -747,11 +762,32 @@
       <c r="B7" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="D7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>46</v>
+      </c>
       <c r="Q7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>21</v>
@@ -766,7 +802,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>14</v>
@@ -778,7 +814,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>21</v>
@@ -787,7 +823,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>13</v>
@@ -799,10 +835,10 @@
         <v>15</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>26</v>
@@ -811,28 +847,28 @@
         <v>17</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="Q9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>13</v>
@@ -850,7 +886,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>21</v>
@@ -877,7 +913,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>21</v>
@@ -886,13 +922,13 @@
         <v>31</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>14</v>
@@ -901,13 +937,13 @@
         <v>15</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="Q12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>34</v>
@@ -916,16 +952,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>13</v>
@@ -934,13 +970,13 @@
         <v>13</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="N14" s="0" t="s">
         <v>26</v>
@@ -949,30 +985,30 @@
         <v>17</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="E15" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>14</v>
@@ -987,7 +1023,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>21</v>
@@ -996,37 +1032,37 @@
         <v>31</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>15</v>
       </c>
       <c r="I16" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>65</v>
       </c>
       <c r="Q16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>33</v>
@@ -1050,13 +1086,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>13</v>
@@ -1065,7 +1101,7 @@
         <v>33</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>15</v>
@@ -1074,7 +1110,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>21</v>
@@ -1083,7 +1119,7 @@
         <v>31</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>21</v>
@@ -1095,19 +1131,19 @@
         <v>15</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="Q19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>34</v>
@@ -1116,7 +1152,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>21</v>
@@ -1125,7 +1161,7 @@
         <v>31</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>13</v>
@@ -1134,13 +1170,13 @@
         <v>13</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="Q21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>21</v>
@@ -1149,7 +1185,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>13</v>
@@ -1161,14 +1197,14 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>21</v>
@@ -1180,7 +1216,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
@@ -1192,7 +1228,7 @@
     </row>
     <row r="25" customFormat="false" ht="23.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -1221,8 +1257,8 @@
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1250,31 +1286,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>14</v>
@@ -1286,7 +1322,7 @@
         <v>17</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>28</v>
@@ -1379,6 +1415,15 @@
       <c r="A7" s="14" t="s">
         <v>40</v>
       </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="O7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1389,7 +1434,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -1413,7 +1458,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -1428,7 +1473,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -1449,7 +1494,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
@@ -1469,7 +1514,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1</v>
@@ -1496,13 +1541,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="O14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -1523,7 +1568,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
@@ -1550,7 +1595,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
@@ -1574,7 +1619,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -1595,7 +1640,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
@@ -1613,7 +1658,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
@@ -1631,13 +1676,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="O21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -1655,7 +1700,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
@@ -1673,7 +1718,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B24" s="7" t="n">
         <v>1</v>
@@ -1698,7 +1743,7 @@
       <c r="A25" s="15"/>
       <c r="B25" s="16" t="n">
         <f aca="false">SUM(B2:B24)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C25" s="16" t="n">
         <f aca="false">SUM(C3:C24)</f>
@@ -1706,7 +1751,7 @@
       </c>
       <c r="D25" s="16" t="n">
         <f aca="false">SUM(D3:D24)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E25" s="16" t="n">
         <f aca="false">SUM(E3:E24)</f>
@@ -1735,7 +1780,7 @@
       </c>
       <c r="L25" s="16" t="n">
         <f aca="false">SUM(L2:L24)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M25" s="16" t="n">
         <f aca="false">SUM(M2:M24)</f>
@@ -1751,7 +1796,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>

</xml_diff>